<commit_message>
After tests there are 2 generators that are "incomplete": "String" and "date"
</commit_message>
<xml_diff>
--- a/res/CDAVariables.xlsx
+++ b/res/CDAVariables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="336">
   <si>
     <t xml:space="preserve">Datenfeld</t>
   </si>
@@ -303,10 +303,13 @@
     <t xml:space="preserve">SELF</t>
   </si>
   <si>
+    <t xml:space="preserve">String_test</t>
+  </si>
+  <si>
     <t xml:space="preserve">value_set=[FAMDEP,SELF]</t>
   </si>
   <si>
-    <t xml:space="preserve">displayname</t>
+    <t xml:space="preserve">If FAMDEP then AssociatedPerson</t>
   </si>
   <si>
     <t xml:space="preserve">?</t>
@@ -482,6 +485,9 @@
     <t xml:space="preserve">KV-Notdienst außerhalb des Krankenhauses</t>
   </si>
   <si>
+    <t xml:space="preserve">displayname</t>
+  </si>
+  <si>
     <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@displayName</t>
   </si>
   <si>
@@ -641,6 +647,30 @@
     <t xml:space="preserve">1.2.276.0.76.5.438</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">value_set=[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1.2.276.0.76.5.438]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicht fertig</t>
+  </si>
+  <si>
     <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
   </si>
   <si>
@@ -740,37 +770,40 @@
     <t xml:space="preserve">37637-6</t>
   </si>
   <si>
-    <t xml:space="preserve">regex=^\d{5}-\d$</t>
+    <t xml:space="preserve">regex=\d{5}-\d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockweise Generieren, REGEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0..n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik  displayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_display_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extremity X-ray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik Zeitpunkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201501171650</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise Generieren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0..n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik  displayName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_display_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extremity X-ray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik Zeitpunkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">201501171650</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
@@ -1027,7 +1060,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1078,6 +1111,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1362,8 +1401,8 @@
   </sheetPr>
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E44" activeCellId="0" sqref="E44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1373,7 +1412,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="66.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="45.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="112.75"/>
@@ -1825,27 +1864,27 @@
         <v>92</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>987654321</v>
@@ -1854,48 +1893,48 @@
         <v>30</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
@@ -1907,18 +1946,18 @@
         <v>32</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>19</v>
@@ -1930,18 +1969,18 @@
         <v>32</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>19</v>
@@ -1953,18 +1992,18 @@
         <v>32</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>19</v>
@@ -1976,18 +2015,18 @@
         <v>32</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>19</v>
@@ -1999,47 +2038,47 @@
         <v>21</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>60</v>
@@ -2048,24 +2087,24 @@
         <v>32</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>60</v>
@@ -2074,15 +2113,15 @@
         <v>21</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>3</v>
@@ -2091,30 +2130,30 @@
         <v>30</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>32</v>
@@ -2123,64 +2162,64 @@
         <v>14</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>37</v>
@@ -2189,70 +2228,70 @@
         <v>32</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>37</v>
@@ -2262,48 +2301,48 @@
         <v>32</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>37</v>
@@ -2313,163 +2352,168 @@
         <v>21</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="G44" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>21</v>
@@ -2478,24 +2522,24 @@
         <v>38</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>32</v>
@@ -2504,15 +2548,15 @@
         <v>38</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>13</v>
@@ -2528,24 +2572,24 @@
         <v>38</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>32</v>
@@ -2554,24 +2598,24 @@
         <v>38</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>32</v>
@@ -2580,24 +2624,24 @@
         <v>38</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>32</v>
@@ -2606,18 +2650,18 @@
         <v>38</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>37</v>
@@ -2627,162 +2671,162 @@
         <v>21</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>37</v>
@@ -2795,69 +2839,69 @@
         <v>38</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>174</v>
@@ -2866,25 +2910,25 @@
         <v>30</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="C62" s="2" t="n">
         <v>174</v>
@@ -2893,196 +2937,196 @@
         <v>30</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="7" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>60</v>
@@ -3091,27 +3135,27 @@
         <v>13</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="7" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>60</v>
@@ -3120,27 +3164,27 @@
         <v>13</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>296</v>
-      </c>
       <c r="D71" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>60</v>
@@ -3149,27 +3193,27 @@
         <v>13</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="7" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>60</v>
@@ -3178,51 +3222,51 @@
         <v>13</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>32</v>
@@ -3231,24 +3275,24 @@
         <v>38</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>32</v>
@@ -3257,24 +3301,24 @@
         <v>38</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="D76" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>32</v>
@@ -3283,24 +3327,24 @@
         <v>38</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>32</v>
@@ -3309,18 +3353,18 @@
         <v>38</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>37</v>
@@ -3333,18 +3377,18 @@
         <v>38</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>37</v>
@@ -3354,37 +3398,37 @@
         <v>32</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add parser for Constraints
</commit_message>
<xml_diff>
--- a/res/CDAVariables.xlsx
+++ b/res/CDAVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DC880D-D385-45DD-ACFF-27AB65892B4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDDA739-07F0-4E19-B9D3-AF329D8B4FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="348">
   <si>
     <t>Concept Id</t>
   </si>
@@ -992,9 +992,6 @@
   </si>
   <si>
     <t>fehlerfrei</t>
-  </si>
-  <si>
-    <t>asd</t>
   </si>
   <si>
     <t>period</t>
@@ -1353,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1377,7 +1374,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1386,13 +1383,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>316</v>
@@ -1424,7 +1421,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="1" t="s">
@@ -1448,7 +1445,7 @@
         <v>26</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="6"/>
@@ -1476,7 +1473,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="6"/>
@@ -1504,7 +1501,7 @@
         <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G5" s="1"/>
       <c r="I5" s="1" t="s">
@@ -1531,7 +1528,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G6" s="1"/>
       <c r="I6" s="1" t="s">
@@ -1555,7 +1552,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G7" s="1"/>
       <c r="I7" s="1" t="s">
@@ -1629,7 +1626,7 @@
         <v>265</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="6"/>
@@ -1683,7 +1680,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G12" s="1"/>
       <c r="I12" s="1" t="s">
@@ -1710,7 +1707,7 @@
         <v>26</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="6"/>
@@ -1765,7 +1762,7 @@
         <v>26</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>318</v>
@@ -1824,7 +1821,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G17" s="1"/>
       <c r="I17" s="1" t="s">
@@ -1848,7 +1845,7 @@
         <v>26</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G18" s="1"/>
       <c r="I18" s="1" t="s">
@@ -1875,7 +1872,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G19" s="1"/>
       <c r="I19" s="1" t="s">
@@ -1902,7 +1899,7 @@
         <v>26</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="6"/>
@@ -1930,7 +1927,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G21" s="1"/>
       <c r="I21" s="1" t="s">
@@ -1954,7 +1951,7 @@
         <v>16</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>317</v>
@@ -1983,7 +1980,7 @@
         <v>16</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
@@ -2013,7 +2010,7 @@
         <v>16</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G24" s="1"/>
       <c r="I24" s="1" t="s">
@@ -2040,7 +2037,7 @@
         <v>16</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G25" s="1"/>
       <c r="I25" s="1" t="s">
@@ -2064,7 +2061,7 @@
         <v>16</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G26" s="1"/>
       <c r="I26" s="1" t="s">
@@ -2085,13 +2082,13 @@
         <v>112</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G27" s="1"/>
       <c r="I27" s="1" t="s">
@@ -2112,13 +2109,13 @@
         <v>116</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G28" s="1"/>
       <c r="I28" s="1" t="s">
@@ -2139,13 +2136,13 @@
         <v>108</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G29" s="1"/>
       <c r="I29" s="1" t="s">
@@ -2166,13 +2163,13 @@
         <v>181</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="G30" s="1"/>
       <c r="I30" s="1" t="s">
@@ -2193,13 +2190,13 @@
         <v>185</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="G31" s="1"/>
       <c r="I31" s="1" t="s">
@@ -2305,7 +2302,7 @@
         <v>26</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1" t="s">
@@ -2332,7 +2329,7 @@
         <v>26</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G36" s="1"/>
       <c r="I36" s="1" t="s">
@@ -2356,7 +2353,7 @@
         <v>26</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="6"/>
@@ -2384,7 +2381,7 @@
         <v>26</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="6"/>
@@ -2412,7 +2409,7 @@
         <v>26</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="6"/>
@@ -2440,7 +2437,7 @@
         <v>26</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="6"/>
@@ -2468,7 +2465,7 @@
         <v>26</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="6"/>
@@ -3489,11 +3486,6 @@
       </c>
       <c r="K80" s="1" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2">
-      <c r="B81" s="1" t="s">
-        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Phase2 Dependecy calculation  for Dates only so far
</commit_message>
<xml_diff>
--- a/res/CDAVariables.xlsx
+++ b/res/CDAVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABB3948-BAD2-49FC-B117-48E9D20DBDBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD23941C-1E8A-4039-B7A6-F032DA854CFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$L$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$K$81</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="349">
   <si>
     <t>Concept Id</t>
   </si>
@@ -994,24 +994,9 @@
     <t>fehlerfrei</t>
   </si>
   <si>
-    <t>period</t>
-  </si>
-  <si>
     <t>format=yyyymmddhhmm</t>
   </si>
   <si>
-    <t>Constraints</t>
-  </si>
-  <si>
-    <t>interval=[triage_ts_start,entlassung_ts]</t>
-  </si>
-  <si>
-    <t>min=aufnahme_ts;range=10min</t>
-  </si>
-  <si>
-    <t>min=arztkontakt_ts;range=10min</t>
-  </si>
-  <si>
     <t>format=yyyymmdd;start_date=19200101;end_date=20200730</t>
   </si>
   <si>
@@ -1075,14 +1060,32 @@
     <t>Variable name</t>
   </si>
   <si>
-    <t>interval=[aufnahme_ts,entlassung_ts]</t>
+    <t>_aufnahme_therapiebeginn</t>
+  </si>
+  <si>
+    <t>scope=10-120</t>
+  </si>
+  <si>
+    <t>_therapiebeginn_arztkontakt</t>
+  </si>
+  <si>
+    <t>_arztkontakt_endarztkontakt</t>
+  </si>
+  <si>
+    <t>_endarztkontakt_entlassung</t>
+  </si>
+  <si>
+    <t>_triagestart_triageend</t>
+  </si>
+  <si>
+    <t>_entlassung_triagestart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1115,6 +1118,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1350,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1362,19 +1371,18 @@
     <col min="2" max="2" width="25.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.25" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="66.25" customWidth="1"/>
-    <col min="7" max="7" width="10.75" customWidth="1"/>
-    <col min="8" max="8" width="45.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="1"/>
-    <col min="10" max="10" width="12.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="112.75" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="66.25" customWidth="1"/>
+    <col min="6" max="6" width="10.75" customWidth="1"/>
+    <col min="7" max="7" width="45.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="1"/>
+    <col min="9" max="9" width="12.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="112.75" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="3" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1383,31 +1391,28 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>344</v>
+        <v>316</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>316</v>
+        <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>132</v>
       </c>
@@ -1420,18 +1425,18 @@
       <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>258</v>
       </c>
@@ -1444,22 +1449,22 @@
       <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="6"/>
+      <c r="E3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I3" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K3" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>260</v>
       </c>
@@ -1472,22 +1477,22 @@
       <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="6"/>
+      <c r="E4" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I4" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K4" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -1500,21 +1505,21 @@
       <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="G5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I5" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
@@ -1527,18 +1532,18 @@
       <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="I6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="H6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -1551,18 +1556,18 @@
       <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="I7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="H7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>292</v>
       </c>
@@ -1575,19 +1580,19 @@
       <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="H8" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="I8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>175</v>
       </c>
@@ -1600,19 +1605,19 @@
       <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="H9" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="I9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>262</v>
       </c>
@@ -1625,22 +1630,22 @@
       <c r="D10" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="6"/>
+      <c r="E10" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I10" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K10" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1653,20 +1658,20 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H11" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>204</v>
       </c>
@@ -1679,21 +1684,21 @@
       <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="G12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I12" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:10">
       <c r="A13" s="6" t="s">
         <v>274</v>
       </c>
@@ -1706,22 +1711,22 @@
       <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="6"/>
+      <c r="E13" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I13" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K13" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>190</v>
       </c>
@@ -1734,21 +1739,21 @@
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="H14" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="I14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1761,23 +1766,23 @@
       <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="F15" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="G15" s="1" t="s">
         <v>318</v>
       </c>
+      <c r="H15" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I15" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1790,24 +1795,24 @@
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>319</v>
+      </c>
       <c r="G16" s="1" t="s">
-        <v>319</v>
+        <v>9</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -1820,18 +1825,18 @@
       <c r="D17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="I17" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>159</v>
       </c>
@@ -1844,21 +1849,21 @@
       <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="G18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I18" s="1" t="s">
-        <v>27</v>
+        <v>157</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K18" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
         <v>215</v>
       </c>
@@ -1871,21 +1876,21 @@
       <c r="D19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="G19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I19" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:10">
       <c r="A20" s="6" t="s">
         <v>271</v>
       </c>
@@ -1898,22 +1903,22 @@
       <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="6"/>
+      <c r="E20" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I20" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K20" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
@@ -1926,18 +1931,18 @@
       <c r="D21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="I21" s="1" t="s">
+      <c r="E21" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="H21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -1950,23 +1955,23 @@
       <c r="D22" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="F22" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G22" s="1" t="s">
         <v>317</v>
       </c>
+      <c r="H22" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I22" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>235</v>
       </c>
@@ -1979,24 +1984,24 @@
       <c r="D23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="H23" s="1" t="s">
-        <v>238</v>
+        <v>27</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>27</v>
+        <v>229</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K23" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>154</v>
       </c>
@@ -2009,21 +2014,21 @@
       <c r="D24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="G24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I24" s="1" t="s">
-        <v>17</v>
+        <v>157</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K24" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>103</v>
       </c>
@@ -2036,18 +2041,18 @@
       <c r="D25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="I25" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="H25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>99</v>
       </c>
@@ -2060,18 +2065,18 @@
       <c r="D26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="I26" s="1" t="s">
+      <c r="E26" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="H26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>110</v>
       </c>
@@ -2082,23 +2087,20 @@
         <v>112</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>320</v>
+        <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="G27" s="1"/>
-      <c r="I27" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="H27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
         <v>114</v>
       </c>
@@ -2109,23 +2111,20 @@
         <v>116</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>320</v>
+        <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="I28" s="1" t="s">
+      <c r="F28" s="1"/>
+      <c r="H28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30">
+    <row r="29" spans="1:10" ht="30">
       <c r="A29" s="1" t="s">
         <v>106</v>
       </c>
@@ -2136,23 +2135,20 @@
         <v>108</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>320</v>
+        <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="I29" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="H29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K29" s="7" t="s">
+      <c r="J29" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
         <v>179</v>
       </c>
@@ -2163,23 +2159,20 @@
         <v>181</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="G30" s="1"/>
-      <c r="I30" s="1" t="s">
+      <c r="F30" s="1"/>
+      <c r="H30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
         <v>183</v>
       </c>
@@ -2190,23 +2183,20 @@
         <v>185</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="G31" s="1"/>
-      <c r="I31" s="1" t="s">
+      <c r="F31" s="1"/>
+      <c r="H31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>163</v>
       </c>
@@ -2219,19 +2209,19 @@
       <c r="D32" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I32" s="1" t="s">
-        <v>27</v>
+        <v>157</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K32" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="16.5" customHeight="1">
+    <row r="33" spans="1:10" ht="16.5" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>224</v>
       </c>
@@ -2244,24 +2234,24 @@
       <c r="D33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="G33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="H33" s="1" t="s">
-        <v>228</v>
+        <v>27</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>27</v>
+        <v>229</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K33" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
         <v>217</v>
       </c>
@@ -2274,21 +2264,21 @@
       <c r="D34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I34" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K34" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
         <v>123</v>
       </c>
@@ -2301,21 +2291,21 @@
       <c r="D35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="G35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H35" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
         <v>187</v>
       </c>
@@ -2328,18 +2318,18 @@
       <c r="D36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="I36" s="1" t="s">
+      <c r="E36" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="H36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
         <v>251</v>
       </c>
@@ -2352,22 +2342,22 @@
       <c r="D37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="6"/>
+      <c r="E37" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I37" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K37" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:10">
       <c r="A38" s="6" t="s">
         <v>276</v>
       </c>
@@ -2380,22 +2370,22 @@
       <c r="D38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="6"/>
+      <c r="E38" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I38" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K38" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
         <v>255</v>
       </c>
@@ -2408,22 +2398,22 @@
       <c r="D39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="6"/>
+      <c r="E39" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I39" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K39" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
         <v>266</v>
       </c>
@@ -2436,22 +2426,22 @@
       <c r="D40" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="6"/>
+      <c r="E40" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I40" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K40" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
         <v>269</v>
       </c>
@@ -2464,22 +2454,22 @@
       <c r="D41" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="6"/>
+      <c r="E41" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I41" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K41" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
         <v>118</v>
       </c>
@@ -2492,18 +2482,18 @@
       <c r="D42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="I42" s="1" t="s">
+      <c r="F42" s="1"/>
+      <c r="H42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
         <v>150</v>
       </c>
@@ -2516,14 +2506,14 @@
       <c r="D43" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:10">
       <c r="A44" s="6" t="s">
         <v>289</v>
       </c>
@@ -2536,24 +2526,24 @@
       <c r="D44" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="6" t="s">
+      <c r="F44" s="1"/>
+      <c r="G44" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="H44" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I44" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K44" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
         <v>145</v>
       </c>
@@ -2566,14 +2556,14 @@
       <c r="D45" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:10">
       <c r="A46" s="6" t="s">
         <v>283</v>
       </c>
@@ -2586,24 +2576,24 @@
       <c r="D46" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="6" t="s">
+      <c r="F46" s="1"/>
+      <c r="G46" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="H46" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I46" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K46" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:10">
       <c r="A47" s="6" t="s">
         <v>279</v>
       </c>
@@ -2616,24 +2606,24 @@
       <c r="D47" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="G47" s="1"/>
-      <c r="H47" s="6" t="s">
+      <c r="F47" s="1"/>
+      <c r="G47" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="H47" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I47" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K47" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:10">
       <c r="A48" s="6" t="s">
         <v>286</v>
       </c>
@@ -2646,24 +2636,24 @@
       <c r="D48" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="6" t="s">
+      <c r="F48" s="1"/>
+      <c r="G48" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="H48" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I48" s="1" t="s">
-        <v>10</v>
+        <v>229</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K48" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
         <v>29</v>
       </c>
@@ -2676,19 +2666,19 @@
       <c r="D49" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="H49" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I49" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K49" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
         <v>167</v>
       </c>
@@ -2701,22 +2691,22 @@
       <c r="D50" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="G50" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="H50" s="1" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>17</v>
+        <v>157</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K50" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
         <v>306</v>
       </c>
@@ -2729,19 +2719,19 @@
       <c r="D51" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="H51" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I51" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K51" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -2754,16 +2744,16 @@
       <c r="D52" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="I52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
         <v>171</v>
       </c>
@@ -2776,16 +2766,16 @@
       <c r="D53" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="I53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="J53" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
         <v>231</v>
       </c>
@@ -2798,22 +2788,22 @@
       <c r="D54" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
+      <c r="G54" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="H54" s="1" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>17</v>
+        <v>229</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K54" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
         <v>208</v>
       </c>
@@ -2826,21 +2816,21 @@
       <c r="D55" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="H55" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I55" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K55" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
         <v>300</v>
       </c>
@@ -2853,21 +2843,21 @@
       <c r="D56" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="H56" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I56" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K56" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
         <v>208</v>
       </c>
@@ -2880,19 +2870,19 @@
       <c r="D57" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="H57" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I57" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K57" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:10">
       <c r="A58" s="1" t="s">
         <v>46</v>
       </c>
@@ -2905,19 +2895,19 @@
       <c r="D58" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="H58" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I58" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K58" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
         <v>135</v>
       </c>
@@ -2930,21 +2920,21 @@
       <c r="D59" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F59" s="8" t="s">
+      <c r="E59" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="G59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="H59" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I59" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K59" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
         <v>140</v>
       </c>
@@ -2957,21 +2947,21 @@
       <c r="D60" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="E60" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="G60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="H60" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="I60" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:10">
       <c r="A61" s="1" t="s">
         <v>50</v>
       </c>
@@ -2984,21 +2974,21 @@
       <c r="D61" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H61" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I61" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="J61" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:10">
       <c r="A62" s="1" t="s">
         <v>68</v>
       </c>
@@ -3011,16 +3001,16 @@
       <c r="D62" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="I62" s="1" t="s">
+      <c r="H62" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K62" s="1" t="s">
+      <c r="J62" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:10">
       <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
@@ -3033,19 +3023,19 @@
       <c r="D63" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+      <c r="H63" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I63" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K63" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:10">
       <c r="A64" s="1" t="s">
         <v>248</v>
       </c>
@@ -3058,19 +3048,19 @@
       <c r="D64" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
+      <c r="H64" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I64" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K64" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:10">
       <c r="A65" s="1" t="s">
         <v>196</v>
       </c>
@@ -3083,19 +3073,19 @@
       <c r="D65" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
+      <c r="G65" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="H65" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="I65" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="J65" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:10">
       <c r="A66" s="1" t="s">
         <v>244</v>
       </c>
@@ -3108,22 +3098,22 @@
       <c r="D66" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E66" s="1"/>
       <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
+      <c r="G66" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="H66" s="1" t="s">
-        <v>238</v>
+        <v>17</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>17</v>
+        <v>229</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K66" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:10">
       <c r="A67" s="1" t="s">
         <v>240</v>
       </c>
@@ -3136,24 +3126,24 @@
       <c r="D67" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="G67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="H67" s="1" t="s">
-        <v>238</v>
+        <v>27</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>27</v>
+        <v>229</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K67" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:10">
       <c r="A68" s="1" t="s">
         <v>200</v>
       </c>
@@ -3166,22 +3156,22 @@
       <c r="D68" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
+      <c r="G68" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="H68" s="1" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K68" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:10">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
@@ -3194,16 +3184,16 @@
       <c r="D69" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="I69" s="1" t="s">
+      <c r="H69" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="J69" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:10">
       <c r="A70" s="1" t="s">
         <v>221</v>
       </c>
@@ -3216,19 +3206,19 @@
       <c r="D70" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
+      <c r="H70" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I70" s="1" t="s">
-        <v>17</v>
+        <v>157</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K70" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:10">
       <c r="A71" s="1" t="s">
         <v>127</v>
       </c>
@@ -3241,21 +3231,21 @@
       <c r="D71" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="E71" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H71" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I71" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K71" s="1" t="s">
+      <c r="J71" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:10">
       <c r="A72" s="1" t="s">
         <v>309</v>
       </c>
@@ -3268,19 +3258,19 @@
       <c r="D72" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
+      <c r="H72" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I72" s="1" t="s">
-        <v>27</v>
+        <v>229</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K72" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:10">
       <c r="A73" s="1" t="s">
         <v>94</v>
       </c>
@@ -3293,19 +3283,19 @@
       <c r="D73" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
+      <c r="G73" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="H73" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I73" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K73" s="1" t="s">
+      <c r="J73" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:10">
       <c r="A74" s="1" t="s">
         <v>83</v>
       </c>
@@ -3318,21 +3308,21 @@
       <c r="D74" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="E74" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="H74" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I74" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="J74" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:10">
       <c r="A75" s="1" t="s">
         <v>79</v>
       </c>
@@ -3345,16 +3335,16 @@
       <c r="D75" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E75" s="1"/>
       <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="I75" s="1" t="s">
+      <c r="H75" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K75" s="1" t="s">
+      <c r="J75" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:10">
       <c r="A76" s="1" t="s">
         <v>42</v>
       </c>
@@ -3367,19 +3357,19 @@
       <c r="D76" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
+      <c r="H76" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I76" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K76" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:10">
       <c r="A77" s="1" t="s">
         <v>296</v>
       </c>
@@ -3392,21 +3382,21 @@
       <c r="D77" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="E77" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="H77" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I77" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K77" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:10">
       <c r="A78" s="1" t="s">
         <v>302</v>
       </c>
@@ -3419,21 +3409,21 @@
       <c r="D78" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="E78" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="H78" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I78" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K78" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:10">
       <c r="A79" s="1" t="s">
         <v>304</v>
       </c>
@@ -3446,21 +3436,21 @@
       <c r="D79" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="E79" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="H79" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I79" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K79" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:10">
       <c r="A80" s="1" t="s">
         <v>313</v>
       </c>
@@ -3473,22 +3463,89 @@
       <c r="D80" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E80" s="1"/>
       <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
+      <c r="G80" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="H80" s="1" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>17</v>
+        <v>229</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K80" s="1" t="s">
         <v>312</v>
       </c>
     </row>
+    <row r="81" spans="2:5">
+      <c r="B81" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5">
+      <c r="B82" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5">
+      <c r="B83" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5">
+      <c r="B84" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5">
+      <c r="B85" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5">
+      <c r="B86" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Generation working for all but String
</commit_message>
<xml_diff>
--- a/res/CDAVariables.xlsx
+++ b/res/CDAVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD23941C-1E8A-4039-B7A6-F032DA854CFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F21461-6C8F-4B95-871F-B48D581D97F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1361,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fehlerfrei bis auf Diagnostik und Associatet Person und Nullflavors; added Valueset for CEDIS und Diagnostik Codes
</commit_message>
<xml_diff>
--- a/res/CDAVariables.xlsx
+++ b/res/CDAVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F21461-6C8F-4B95-871F-B48D581D97F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A36EA5A-5FC7-4B07-9785-F1B948735AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="350">
   <si>
     <t>Concept Id</t>
   </si>
@@ -448,9 +448,6 @@
     <t>KVNDAK</t>
   </si>
   <si>
-    <t>value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINC, NPHYS]</t>
-  </si>
-  <si>
     <t>ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
   </si>
   <si>
@@ -715,9 +712,6 @@
     <t>37637-6</t>
   </si>
   <si>
-    <t>regex=\d{5}-\d</t>
-  </si>
-  <si>
     <t>Blockweise Generieren, REGEX</t>
   </si>
   <si>
@@ -1079,6 +1073,15 @@
   </si>
   <si>
     <t>_entlassung_triagestart</t>
+  </si>
+  <si>
+    <t>link=cedis.csv</t>
+  </si>
+  <si>
+    <t>link=diagnostic_codes.csv</t>
+  </si>
+  <si>
+    <t>value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
   </si>
 </sst>
 </file>
@@ -1361,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1382,7 +1385,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1391,13 +1394,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
@@ -1426,7 +1429,7 @@
         <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="1" t="s">
@@ -1438,10 +1441,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C3" s="2">
         <v>174</v>
@@ -1450,7 +1453,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="6"/>
@@ -1458,18 +1461,18 @@
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C4" s="2">
         <v>174</v>
@@ -1478,7 +1481,7 @@
         <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="6"/>
@@ -1486,10 +1489,10 @@
         <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1506,7 +1509,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F5" s="1"/>
       <c r="H5" s="1" t="s">
@@ -1533,7 +1536,7 @@
         <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F6" s="1"/>
       <c r="H6" s="1" t="s">
@@ -1557,7 +1560,7 @@
         <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F7" s="1"/>
       <c r="H7" s="1" t="s">
@@ -1569,13 +1572,13 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>294</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>32</v>
@@ -1583,24 +1586,24 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>32</v>
@@ -1608,30 +1611,30 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="D10" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="6"/>
@@ -1639,10 +1642,10 @@
         <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1673,19 +1676,19 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F12" s="1"/>
       <c r="H12" s="1" t="s">
@@ -1695,24 +1698,24 @@
         <v>33</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
@@ -1720,37 +1723,37 @@
         <v>10</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1767,10 +1770,10 @@
         <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>27</v>
@@ -1797,7 +1800,7 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>9</v>
@@ -1826,7 +1829,7 @@
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F17" s="1"/>
       <c r="H17" s="1" t="s">
@@ -1838,46 +1841,46 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F18" s="1"/>
       <c r="H18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F19" s="1"/>
       <c r="H19" s="1" t="s">
@@ -1887,24 +1890,24 @@
         <v>33</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="6"/>
@@ -1912,10 +1915,10 @@
         <v>10</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1932,7 +1935,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F21" s="1"/>
       <c r="H21" s="1" t="s">
@@ -1956,10 +1959,10 @@
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>17</v>
@@ -1973,59 +1976,59 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F24" s="1"/>
       <c r="H24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I24" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2042,7 +2045,7 @@
         <v>16</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F25" s="1"/>
       <c r="H25" s="1" t="s">
@@ -2066,7 +2069,7 @@
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F26" s="1"/>
       <c r="H26" s="1" t="s">
@@ -2090,7 +2093,7 @@
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F27" s="1"/>
       <c r="H27" s="1" t="s">
@@ -2114,7 +2117,7 @@
         <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F28" s="1"/>
       <c r="H28" s="1" t="s">
@@ -2138,7 +2141,7 @@
         <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F29" s="1"/>
       <c r="H29" s="1" t="s">
@@ -2150,122 +2153,124 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F30" s="1"/>
       <c r="H30" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F31" s="1"/>
       <c r="H31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="D32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="H32" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="16.5" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="D33" s="1" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>227</v>
+        <v>348</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C34" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="F34" s="1"/>
       <c r="H34" s="1" t="s">
@@ -2275,7 +2280,7 @@
         <v>33</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2292,7 +2297,7 @@
         <v>26</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
@@ -2307,19 +2312,19 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F36" s="1"/>
       <c r="H36" s="1" t="s">
@@ -2331,19 +2336,19 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>253</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="6"/>
@@ -2351,27 +2356,27 @@
         <v>10</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="6"/>
@@ -2379,27 +2384,27 @@
         <v>10</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="6"/>
@@ -2407,27 +2412,27 @@
         <v>10</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="6"/>
@@ -2435,27 +2440,27 @@
         <v>10</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="6"/>
@@ -2463,10 +2468,10 @@
         <v>10</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2495,13 +2500,13 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="C43" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>32</v>
@@ -2510,24 +2515,24 @@
         <v>27</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="D44" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="6" t="s">
@@ -2537,47 +2542,47 @@
         <v>10</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G45" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="D46" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="6" t="s">
@@ -2587,27 +2592,27 @@
         <v>10</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="D47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="6" t="s">
@@ -2617,27 +2622,27 @@
         <v>10</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="6" t="s">
@@ -2647,10 +2652,10 @@
         <v>10</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2680,13 +2685,13 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>32</v>
@@ -2694,27 +2699,27 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>308</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>32</v>
@@ -2728,7 +2733,7 @@
         <v>33</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2755,13 +2760,13 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>32</v>
@@ -2772,18 +2777,18 @@
         <v>17</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>233</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>32</v>
@@ -2791,33 +2796,33 @@
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="F55" s="1"/>
       <c r="H55" s="1" t="s">
@@ -2827,24 +2832,24 @@
         <v>33</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="F56" s="1"/>
       <c r="H56" s="1" t="s">
@@ -2854,15 +2859,15 @@
         <v>33</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>10</v>
@@ -2879,7 +2884,7 @@
         <v>33</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2921,7 +2926,7 @@
         <v>32</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>138</v>
+        <v>349</v>
       </c>
       <c r="F59" s="8"/>
       <c r="H59" s="1" t="s">
@@ -2931,34 +2936,34 @@
         <v>11</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="D60" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>138</v>
+        <v>349</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -3037,13 +3042,13 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>248</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>250</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>32</v>
@@ -3057,18 +3062,18 @@
         <v>33</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>32</v>
@@ -3076,24 +3081,24 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>32</v>
@@ -3101,57 +3106,57 @@
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="D67" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>32</v>
@@ -3159,7 +3164,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>17</v>
@@ -3168,7 +3173,7 @@
         <v>33</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -3195,13 +3200,13 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>32</v>
@@ -3212,10 +3217,10 @@
         <v>17</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -3247,13 +3252,13 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>32</v>
@@ -3264,10 +3269,10 @@
         <v>27</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -3371,19 +3376,19 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="D77" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F77" s="1"/>
       <c r="H77" s="1" t="s">
@@ -3393,24 +3398,24 @@
         <v>33</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F78" s="1"/>
       <c r="H78" s="1" t="s">
@@ -3420,24 +3425,24 @@
         <v>33</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F79" s="1"/>
       <c r="H79" s="1" t="s">
@@ -3447,18 +3452,18 @@
         <v>33</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>32</v>
@@ -3466,82 +3471,82 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="81" spans="2:5">
       <c r="B81" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="82" spans="2:5">
       <c r="B82" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="83" spans="2:5">
       <c r="B83" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="84" spans="2:5">
       <c r="B84" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="86" spans="2:5">
       <c r="B86" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>